<commit_message>
Period Slots (Finds spots for all courses)
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c0ad513c21b2b58/Documents/Programming/Python/Schedular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1605" documentId="8_{ABCCCFCC-F580-419F-9EB4-1F0A78ED5454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{586127ED-A837-4EBD-AE93-13B08D5EDD53}"/>
+  <xr:revisionPtr revIDLastSave="1631" documentId="8_{ABCCCFCC-F580-419F-9EB4-1F0A78ED5454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78A9B572-8ADE-4AA2-8138-F3ED33EF96EA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{73A0230C-F103-4711-878E-970B55EAFC2C}"/>
   </bookViews>
@@ -17,8 +17,9 @@
     <sheet name="Teachers" sheetId="3" r:id="rId2"/>
     <sheet name="Rooms" sheetId="4" r:id="rId3"/>
     <sheet name="Courses" sheetId="2" r:id="rId4"/>
-    <sheet name="Duties" sheetId="6" r:id="rId5"/>
-    <sheet name="_Select" sheetId="5" r:id="rId6"/>
+    <sheet name="Grades" sheetId="8" r:id="rId5"/>
+    <sheet name="Duties" sheetId="6" r:id="rId6"/>
+    <sheet name="_Select" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Courses!$A$1:$K$11</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -241,6 +242,12 @@
   </si>
   <si>
     <t>Grades</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>PE</t>
   </si>
 </sst>
 </file>
@@ -329,10 +336,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -655,7 +658,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="XEB1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="XFD22" sqref="XFD22"/>
     </sheetView>
   </sheetViews>
@@ -827,10 +830,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135D99AC-01B5-40E4-99A8-A5007C5B3DE5}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,31 +841,40 @@
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>201</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>202</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>203</v>
       </c>
@@ -870,15 +882,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>205</v>
       </c>
@@ -886,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>204</v>
       </c>
@@ -894,7 +909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>206</v>
       </c>
@@ -902,12 +917,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +939,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,6 +1253,41 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E7822F-BDA8-4A81-B0BA-70E8C1B7B26B}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9B1AE3-C87F-4073-A141-D486FF9852A3}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C6"/>
@@ -1290,7 +1343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB490DB5-7996-45C1-9F7A-896BDD894625}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C3"/>

</xml_diff>

<commit_message>
Fixed + Subdividing into Files
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
   <si>
     <t>Core</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>ALL</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Any</t>
@@ -304,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -324,26 +321,14 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -668,13 +653,13 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -683,38 +668,38 @@
       <c r="B3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1"/>
     </row>
@@ -746,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
@@ -754,79 +739,79 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +830,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
@@ -855,7 +840,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>14</v>
@@ -866,10 +851,10 @@
         <v>201</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -877,10 +862,10 @@
         <v>202</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -888,21 +873,21 @@
         <v>203</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="13" t="s">
-        <v>29</v>
+      <c r="A5" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -910,10 +895,10 @@
         <v>205</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -921,10 +906,10 @@
         <v>204</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -932,21 +917,21 @@
         <v>206</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="13" t="s">
-        <v>49</v>
+      <c r="A9" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -970,8 +955,8 @@
     <col min="3" max="3" style="2" width="36.14785714285715" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="13.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="13.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -993,7 +978,7 @@
       <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1013,45 +998,43 @@
       <c r="E2" s="5">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>8</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
+      <c r="F3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -1059,22 +1042,22 @@
       <c r="E4" s="5">
         <v>8</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
+      <c r="F4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -1082,45 +1065,45 @@
       <c r="E5" s="5">
         <v>8</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
+      <c r="F5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>8</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
+      <c r="F6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>2</v>
@@ -1128,19 +1111,19 @@
       <c r="E7" s="5">
         <v>8</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>21</v>
+      <c r="F7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -1152,16 +1135,16 @@
         <v>8</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
+      <c r="G8" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
@@ -1173,16 +1156,16 @@
         <v>8</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="1" t="s">
-        <v>21</v>
+      <c r="G9" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>
@@ -1194,16 +1177,16 @@
         <v>8</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="10">
+      <c r="G10" s="5">
         <v>206</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
@@ -1215,65 +1198,65 @@
         <v>8</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
+      <c r="G11" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
@@ -1281,22 +1264,22 @@
       <c r="E14" s="5">
         <v>8</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>21</v>
+      <c r="F14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>2</v>
@@ -1304,11 +1287,11 @@
       <c r="E15" s="5">
         <v>8</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>21</v>
+      <c r="F15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1340,10 +1323,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>7</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Random else: return False
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -249,7 +249,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +267,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -330,13 +336,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -345,7 +351,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">

</xml_diff>

<commit_message>
Simplified Same Class Period Slots
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Info"/>
@@ -276,7 +276,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,12 +294,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -346,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -387,13 +381,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -728,16 +716,16 @@
       <c r="B3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -778,7 +766,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -930,7 +918,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="16.433571428571426" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
@@ -1123,7 +1111,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="14"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
@@ -1139,7 +1127,7 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1147,9 +1135,9 @@
     <col min="2" max="2" style="2" width="12.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="33.57642857142857" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="13.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.290714285714287" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
@@ -1662,9 +1650,9 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="14"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="14"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>

</xml_diff>